<commit_message>
Updated borders of the board
</commit_message>
<xml_diff>
--- a/Pacman_board.xlsx
+++ b/Pacman_board.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dennis\Documents\Personal\Projects\PacmanAlgo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEC0170-8A09-45DC-BDB5-E4614090F9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8372DC0-CAFB-4074-97CB-16DD8BB6FB79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-855" windowWidth="29040" windowHeight="15720" xr2:uid="{7101D0AE-20E9-4ADB-A1B2-720EE1E4C0AD}"/>
   </bookViews>
@@ -430,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E6E7326-4F59-45E5-A5CB-4E6B35C1FAE9}">
   <dimension ref="D3:BG23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:BG23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -653,10 +653,10 @@
         <v>1</v>
       </c>
       <c r="O7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q7" t="s">
         <v>1</v>
@@ -671,7 +671,7 @@
         <v>1</v>
       </c>
       <c r="U7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V7" t="s">
         <v>0</v>
@@ -823,13 +823,13 @@
         <v>1</v>
       </c>
       <c r="O8" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R8" t="s">
         <v>0</v>
@@ -838,10 +838,10 @@
         <v>0</v>
       </c>
       <c r="T8" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V8" t="s">
         <v>0</v>
@@ -993,10 +993,10 @@
         <v>1</v>
       </c>
       <c r="O9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q9" t="s">
         <v>0</v>
@@ -1008,10 +1008,10 @@
         <v>0</v>
       </c>
       <c r="T9" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V9" t="s">
         <v>0</v>
@@ -1175,7 +1175,7 @@
         <v>0</v>
       </c>
       <c r="S10" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T10" t="s">
         <v>1</v>
@@ -1342,13 +1342,13 @@
         <v>0</v>
       </c>
       <c r="R11" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S11" t="s">
         <v>1</v>
       </c>
       <c r="T11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U11" t="s">
         <v>0</v>
@@ -1515,7 +1515,7 @@
         <v>1</v>
       </c>
       <c r="S12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T12" t="s">
         <v>0</v>
@@ -1855,7 +1855,7 @@
         <v>1</v>
       </c>
       <c r="S14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T14" t="s">
         <v>0</v>
@@ -2022,13 +2022,13 @@
         <v>0</v>
       </c>
       <c r="R15" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S15" t="s">
         <v>1</v>
       </c>
       <c r="T15" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U15" t="s">
         <v>0</v>
@@ -2195,7 +2195,7 @@
         <v>0</v>
       </c>
       <c r="S16" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T16" t="s">
         <v>1</v>
@@ -2353,10 +2353,10 @@
         <v>1</v>
       </c>
       <c r="O17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q17" t="s">
         <v>0</v>
@@ -2368,10 +2368,10 @@
         <v>0</v>
       </c>
       <c r="T17" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V17" t="s">
         <v>0</v>
@@ -2523,13 +2523,13 @@
         <v>1</v>
       </c>
       <c r="O18" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P18" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q18" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R18" t="s">
         <v>0</v>
@@ -2538,10 +2538,10 @@
         <v>0</v>
       </c>
       <c r="T18" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U18" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V18" t="s">
         <v>0</v>
@@ -2693,10 +2693,10 @@
         <v>1</v>
       </c>
       <c r="O19" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P19" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q19" t="s">
         <v>1</v>
@@ -2711,7 +2711,7 @@
         <v>1</v>
       </c>
       <c r="U19" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V19" t="s">
         <v>0</v>
@@ -2810,7 +2810,7 @@
         <v>0</v>
       </c>
       <c r="BB19" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC19" t="s">
         <v>0</v>
@@ -2878,10 +2878,10 @@
         <v>0</v>
       </c>
       <c r="T20" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U20" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V20" t="s">
         <v>0</v>
@@ -2929,10 +2929,10 @@
         <v>0</v>
       </c>
       <c r="AK20" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL20" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM20" t="s">
         <v>0</v>
@@ -2980,7 +2980,7 @@
         <v>0</v>
       </c>
       <c r="BB20" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC20" t="s">
         <v>0</v>
@@ -3012,10 +3012,10 @@
         <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" t="s">
         <v>1</v>
@@ -3048,10 +3048,10 @@
         <v>0</v>
       </c>
       <c r="T21" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V21" t="s">
         <v>0</v>
@@ -3099,10 +3099,10 @@
         <v>0</v>
       </c>
       <c r="AK21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL21" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM21" t="s">
         <v>0</v>
@@ -3147,13 +3147,13 @@
         <v>0</v>
       </c>
       <c r="BA21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB21" t="s">
         <v>1</v>
       </c>
       <c r="BC21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BD21" t="s">
         <v>0</v>
@@ -3185,7 +3185,7 @@
         <v>1</v>
       </c>
       <c r="I22" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" t="s">
         <v>1</v>
@@ -3221,7 +3221,7 @@
         <v>1</v>
       </c>
       <c r="U22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V22" t="s">
         <v>0</v>
@@ -3269,7 +3269,7 @@
         <v>0</v>
       </c>
       <c r="AK22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL22" t="s">
         <v>1</v>
@@ -3320,7 +3320,7 @@
         <v>1</v>
       </c>
       <c r="BB22" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC22" t="s">
         <v>1</v>

</xml_diff>